<commit_message>
Create rate card: bangalore-bcd-efgfalse
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/hyperlocal/bangalore/BangaloreBcdEfg.xlsx
+++ b/src/main/resources/excel/hyperlocal/bangalore/BangaloreBcdEfg.xlsx
@@ -1682,8 +1682,8 @@
   <sheetPr/>
   <dimension ref="A1:AA851"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15" customHeight="1"/>
@@ -2024,7 +2024,7 @@
       <c r="G17" s="35"/>
       <c r="H17" s="55"/>
       <c r="I17" s="55">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>

</xml_diff>

<commit_message>
Create rate card: bangalore-bcd-efgfalse (#20)
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/hyperlocal/bangalore/BangaloreBcdEfg.xlsx
+++ b/src/main/resources/excel/hyperlocal/bangalore/BangaloreBcdEfg.xlsx
@@ -1682,8 +1682,8 @@
   <sheetPr/>
   <dimension ref="A1:AA851"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15" customHeight="1"/>
@@ -2024,7 +2024,7 @@
       <c r="G17" s="35"/>
       <c r="H17" s="55"/>
       <c r="I17" s="55">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>

</xml_diff>